<commit_message>
Results to now Val64 to Value N, pre-decouple
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordy\Documents\DEV\col-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF0A35-AF88-4F64-B5C3-DB64B8C1BA59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3AECFF-B1DB-44FA-AAD6-BF4D0158A426}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{94B90FBB-95A3-47C2-B663-BF0DC2F55ED3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{94B90FBB-95A3-47C2-B663-BF0DC2F55ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="1980-2000" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="113">
   <si>
     <t>WRRCD</t>
   </si>
@@ -278,14 +278,6 @@
     <t>K140100</t>
   </si>
   <si>
-    <t>12(121.122.123.124)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>11(111. 112. 113. 114)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>OBJECTID</t>
   </si>
   <si>
@@ -359,10 +351,6 @@
   </si>
   <si>
     <t>VALUE_123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from value 64 to other value numbers </t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>from other value numbers to value 64</t>
@@ -375,13 +363,19 @@
   <si>
     <t>This is a conservation matrix, rows represent consersion from value 64 to other value numbers and columns mean conversion from other value numbers to value 64). Atttention : Please make a difference between 0 ( no change) and null (no conversion between value 64 and other value numbers)</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">from value 64 to other value numbers </t>
+  </si>
+  <si>
+    <t>from other value numbers to value 64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +425,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -469,7 +478,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -497,11 +506,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF9555C-2B28-42A7-8844-199EE45FCD3D}">
-  <dimension ref="A1:AZ84"/>
+  <dimension ref="A1:BF84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,283 +858,309 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
-      <c r="B1" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AB1" s="9" t="s">
+    <row r="1" spans="1:58">
+      <c r="B1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="9"/>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="9"/>
-    </row>
-    <row r="2" spans="1:52" s="2" customFormat="1">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="16"/>
+      <c r="BD1" s="16"/>
+      <c r="BE1" s="16"/>
+      <c r="BF1" s="16"/>
+    </row>
+    <row r="2" spans="1:58" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="13">
         <v>21</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="13">
         <v>22</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="13">
         <v>23</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="13">
         <v>24</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="13">
         <v>31</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="13">
         <v>32</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="13">
         <v>33</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="13">
         <v>41</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="13">
         <v>42</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="13">
         <v>43</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="13">
         <v>44</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="13">
         <v>45</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="13">
         <v>46</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="13">
         <v>61</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="13">
         <v>62</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="13">
         <v>63</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="13">
         <v>64</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="13">
         <v>65</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="13">
         <v>66</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="13">
         <v>67</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="X2" s="2">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>52</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>53</v>
-      </c>
-      <c r="AB2" s="2">
+      <c r="V2" s="13">
+        <v>111</v>
+      </c>
+      <c r="W2" s="13">
+        <v>112</v>
+      </c>
+      <c r="X2" s="13">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="13">
+        <v>114</v>
+      </c>
+      <c r="Z2" s="13">
+        <v>121</v>
+      </c>
+      <c r="AA2" s="13">
+        <v>122</v>
+      </c>
+      <c r="AB2" s="13">
+        <v>123</v>
+      </c>
+      <c r="AC2" s="13">
+        <v>124</v>
+      </c>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13">
         <v>21</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AF2" s="13">
         <v>22</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AG2" s="13">
         <v>23</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AH2" s="13">
         <v>24</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AI2" s="13">
         <v>31</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AJ2" s="13">
         <v>32</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AK2" s="13">
         <v>33</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AL2" s="13">
         <v>41</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AM2" s="13">
         <v>42</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AN2" s="13">
         <v>43</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AO2" s="13">
         <v>44</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AP2" s="13">
         <v>45</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AQ2" s="13">
         <v>46</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AR2" s="13">
         <v>61</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="AS2" s="13">
         <v>62</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AT2" s="13">
         <v>63</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AU2" s="13">
         <v>64</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AV2" s="13">
         <v>65</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AW2" s="13">
         <v>66</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AX2" s="13">
         <v>67</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>51</v>
-      </c>
-      <c r="AY2" s="2">
-        <v>52</v>
-      </c>
-      <c r="AZ2" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52">
+      <c r="AY2" s="13">
+        <v>111</v>
+      </c>
+      <c r="AZ2" s="13">
+        <v>112</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>113</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>114</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>122</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>123</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:58">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:58">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:58">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:58">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:58">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:58">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:58">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:58">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:58">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:58">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:58">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:58">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:58">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1452,8 +1508,8 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="2">
-    <mergeCell ref="B1:Z1"/>
-    <mergeCell ref="AB1:AZ1"/>
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="AL1:BB1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1463,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA99934-01A7-4A8A-9484-6FE12D0651E9}">
-  <dimension ref="A1:AZ84"/>
+  <dimension ref="A1:BF84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1474,283 +1530,288 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:58">
       <c r="B1" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AB1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="9"/>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="9"/>
-    </row>
-    <row r="2" spans="1:52" s="2" customFormat="1">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="AL1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+    </row>
+    <row r="2" spans="1:58" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>21</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>23</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>24</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>31</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>32</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>33</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>41</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>42</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>43</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>44</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>45</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>46</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>61</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>62</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <v>63</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2">
         <v>64</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2">
         <v>65</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2">
         <v>66</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2">
         <v>67</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="X2" s="2">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>52</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>53</v>
-      </c>
-      <c r="AB2" s="2">
+      <c r="V2">
+        <v>111</v>
+      </c>
+      <c r="W2">
+        <v>112</v>
+      </c>
+      <c r="X2">
+        <v>113</v>
+      </c>
+      <c r="Y2">
+        <v>114</v>
+      </c>
+      <c r="Z2">
+        <v>121</v>
+      </c>
+      <c r="AA2">
+        <v>122</v>
+      </c>
+      <c r="AB2">
+        <v>123</v>
+      </c>
+      <c r="AC2">
+        <v>124</v>
+      </c>
+      <c r="AD2"/>
+      <c r="AE2">
         <v>21</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AF2">
         <v>22</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AG2">
         <v>23</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AH2">
         <v>24</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AI2">
         <v>31</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AJ2">
         <v>32</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AK2">
         <v>33</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AL2">
         <v>41</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AM2">
         <v>42</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AN2">
         <v>43</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AO2">
         <v>44</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AP2">
         <v>45</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AQ2">
         <v>46</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AR2">
         <v>61</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="AS2">
         <v>62</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AT2">
         <v>63</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AU2">
         <v>64</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AV2">
         <v>65</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AW2">
         <v>66</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AX2">
         <v>67</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>51</v>
-      </c>
-      <c r="AY2" s="2">
-        <v>52</v>
-      </c>
-      <c r="AZ2" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52">
+      <c r="AY2">
+        <v>111</v>
+      </c>
+      <c r="AZ2">
+        <v>112</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>113</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>114</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>122</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>123</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:58">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:58">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:58">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:58">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:58">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:58">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:58">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:58">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:58">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:58">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:58">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:58">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:58">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2097,11 +2158,12 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:Z1"/>
-    <mergeCell ref="AB1:AZ1"/>
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="AL1:BB1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2125,84 +2187,84 @@
   <sheetData>
     <row r="1" spans="2:26">
       <c r="T1" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="2:26">
       <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>88</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>90</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>91</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>93</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>94</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>95</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>96</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>97</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>98</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>100</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>102</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" t="s">
         <v>103</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>104</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>105</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>106</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>107</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:26">
@@ -3593,7 +3655,7 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1">
         <v>19</v>
@@ -3826,23 +3888,23 @@
       </c>
     </row>
     <row r="25" spans="1:26" s="8" customFormat="1" ht="44.1" customHeight="1">
-      <c r="A25" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="A25" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
     </row>
     <row r="26" spans="1:26" s="8" customFormat="1"/>
   </sheetData>

</xml_diff>